<commit_message>
update new source for changing required
</commit_message>
<xml_diff>
--- a/ui-testsuite/src/main/resources/TestData/ATR_DupliPreviousDoc.xlsx
+++ b/ui-testsuite/src/main/resources/TestData/ATR_DupliPreviousDoc.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Pipeline\Document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Workspace\ui-test\ui-testsuite\src\main\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="221">
   <si>
     <t>IB TYPE</t>
   </si>
@@ -573,9 +573,6 @@
     <t>CE BCRD10</t>
   </si>
   <si>
-    <t>G3</t>
-  </si>
-  <si>
     <t>9443</t>
   </si>
   <si>
@@ -663,69 +660,15 @@
     <t>04/13/2016</t>
   </si>
   <si>
-    <t>2016-Q2</t>
-  </si>
-  <si>
     <t>FUTURE</t>
   </si>
   <si>
     <t>Q3</t>
   </si>
   <si>
-    <t>2152430001</t>
-  </si>
-  <si>
     <t>ADM</t>
   </si>
   <si>
-    <t>5203692434</t>
-  </si>
-  <si>
-    <t>4345065416</t>
-  </si>
-  <si>
-    <t>6554327047</t>
-  </si>
-  <si>
-    <t>7345446630</t>
-  </si>
-  <si>
-    <t>1117780026</t>
-  </si>
-  <si>
-    <t>8452262040</t>
-  </si>
-  <si>
-    <t>8090644094</t>
-  </si>
-  <si>
-    <t>2142597710</t>
-  </si>
-  <si>
-    <t>2820375792</t>
-  </si>
-  <si>
-    <t>3708390204</t>
-  </si>
-  <si>
-    <t>4394704370</t>
-  </si>
-  <si>
-    <t>8258280311</t>
-  </si>
-  <si>
-    <t>3133381113</t>
-  </si>
-  <si>
-    <t>2892964132</t>
-  </si>
-  <si>
-    <t>0488757004</t>
-  </si>
-  <si>
-    <t>9124050564</t>
-  </si>
-  <si>
     <t>0726323960</t>
   </si>
   <si>
@@ -733,6 +676,15 @@
   </si>
   <si>
     <t>2120811097</t>
+  </si>
+  <si>
+    <t>2016-Q3</t>
+  </si>
+  <si>
+    <t>5G</t>
+  </si>
+  <si>
+    <t>8S</t>
   </si>
 </sst>
 </file>
@@ -742,7 +694,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\-yy;@"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -760,66 +712,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="11.0"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="11.0"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="11.0"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="11.0"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="11.0"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="11.0"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="11.0"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="11.0"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="11.0"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="11.0"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="11.0"/>
-      <charset val="0"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <sz val="11.0"/>
-      <charset val="0"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1234,168 +1126,168 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FF3"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BL1" workbookViewId="0">
-      <selection activeCell="BO4" sqref="BO4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AN3" sqref="AN3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="13.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="13.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="12.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="18.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="13.28515625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="47.140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="47.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="32.5703125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" style="1" width="21.0" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="21.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="18" max="19" bestFit="true" customWidth="true" style="1" width="39.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="28.140625" collapsed="true"/>
-    <col min="22" max="23" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="18.5703125" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="12" width="14.7109375" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="12" width="12.7109375" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="2" width="10.5703125" collapsed="true"/>
-    <col min="30" max="30" customWidth="true" style="1" width="19.140625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="12" width="11.85546875" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="12" width="12.7109375" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="2" width="14.5703125" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="19.140625" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="17.42578125" collapsed="true"/>
-    <col min="36" max="37" bestFit="true" customWidth="true" style="10" width="14.140625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" style="1" width="16.140625" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" style="10" width="11.140625" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" style="1" width="14.85546875" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" style="1" width="18.28515625" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" style="1" width="20.85546875" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" style="1" width="12.5703125" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" style="1" width="21.140625" collapsed="true"/>
-    <col min="47" max="48" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" style="1" width="14.140625" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" style="1" width="19.140625" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" style="1" width="21.0" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
-    <col min="55" max="55" bestFit="true" customWidth="true" style="1" width="10.140625" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" style="1" width="15.28515625" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" style="1" width="14.42578125" collapsed="true"/>
-    <col min="58" max="58" bestFit="true" customWidth="true" style="1" width="19.0" collapsed="true"/>
-    <col min="59" max="59" bestFit="true" customWidth="true" style="1" width="18.7109375" collapsed="true"/>
-    <col min="60" max="60" bestFit="true" customWidth="true" style="1" width="19.7109375" collapsed="true"/>
-    <col min="61" max="61" bestFit="true" customWidth="true" style="1" width="19.42578125" collapsed="true"/>
-    <col min="62" max="62" bestFit="true" customWidth="true" style="1" width="22.5703125" collapsed="true"/>
-    <col min="63" max="64" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
-    <col min="65" max="65" bestFit="true" customWidth="true" style="1" width="12.28515625" collapsed="true"/>
-    <col min="66" max="66" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
-    <col min="67" max="67" bestFit="true" customWidth="true" style="1" width="14.28515625" collapsed="true"/>
-    <col min="68" max="68" bestFit="true" customWidth="true" style="1" width="13.0" collapsed="true"/>
-    <col min="69" max="69" bestFit="true" customWidth="true" style="1" width="19.5703125" collapsed="true"/>
-    <col min="70" max="70" bestFit="true" customWidth="true" style="1" width="22.85546875" collapsed="true"/>
-    <col min="71" max="71" bestFit="true" customWidth="true" style="12" width="17.28515625" collapsed="true"/>
-    <col min="72" max="72" bestFit="true" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
-    <col min="73" max="73" bestFit="true" customWidth="true" style="1" width="14.28515625" collapsed="true"/>
-    <col min="74" max="74" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
-    <col min="75" max="75" bestFit="true" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
-    <col min="76" max="76" bestFit="true" customWidth="true" style="1" width="11.85546875" collapsed="true"/>
-    <col min="77" max="77" bestFit="true" customWidth="true" style="1" width="11.5703125" collapsed="true"/>
-    <col min="78" max="78" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="79" max="79" bestFit="true" customWidth="true" style="1" width="10.85546875" collapsed="true"/>
-    <col min="80" max="80" bestFit="true" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
-    <col min="81" max="81" bestFit="true" customWidth="true" style="1" width="25.42578125" collapsed="true"/>
-    <col min="82" max="82" bestFit="true" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
-    <col min="83" max="83" bestFit="true" customWidth="true" style="1" width="13.5703125" collapsed="true"/>
-    <col min="84" max="86" bestFit="true" customWidth="true" style="1" width="30.85546875" collapsed="true"/>
-    <col min="87" max="87" bestFit="true" customWidth="true" style="1" width="22.42578125" collapsed="true"/>
-    <col min="88" max="88" bestFit="true" customWidth="true" style="1" width="39.0" collapsed="true"/>
-    <col min="89" max="89" customWidth="true" style="2" width="14.42578125" collapsed="true"/>
-    <col min="90" max="90" bestFit="true" customWidth="true" style="1" width="17.140625" collapsed="true"/>
-    <col min="91" max="91" bestFit="true" customWidth="true" style="1" width="27.28515625" collapsed="true"/>
-    <col min="92" max="92" bestFit="true" customWidth="true" style="1" width="31.140625" collapsed="true"/>
-    <col min="93" max="93" customWidth="true" style="1" width="24.28515625" collapsed="true"/>
-    <col min="94" max="94" bestFit="true" customWidth="true" style="3" width="9.140625" collapsed="true"/>
-    <col min="95" max="95" bestFit="true" customWidth="true" style="4" width="17.140625" collapsed="true"/>
-    <col min="96" max="96" bestFit="true" customWidth="true" style="4" width="15.5703125" collapsed="true"/>
-    <col min="97" max="97" customWidth="true" style="1" width="24.0" collapsed="true"/>
-    <col min="98" max="98" bestFit="true" customWidth="true" style="1" width="24.7109375" collapsed="true"/>
-    <col min="99" max="99" bestFit="true" customWidth="true" style="4" width="21.42578125" collapsed="true"/>
-    <col min="100" max="100" bestFit="true" customWidth="true" style="4" width="19.7109375" collapsed="true"/>
-    <col min="101" max="101" bestFit="true" customWidth="true" style="1" width="15.85546875" collapsed="true"/>
-    <col min="102" max="102" bestFit="true" customWidth="true" style="1" width="13.85546875" collapsed="true"/>
-    <col min="103" max="103" bestFit="true" customWidth="true" style="1" width="39.42578125" collapsed="true"/>
-    <col min="104" max="104" bestFit="true" customWidth="true" style="1" width="12.140625" collapsed="true"/>
-    <col min="105" max="105" customWidth="true" style="2" width="14.42578125" collapsed="true"/>
-    <col min="106" max="106" bestFit="true" customWidth="true" style="2" width="15.5703125" collapsed="true"/>
-    <col min="107" max="107" bestFit="true" customWidth="true" style="2" width="19.85546875" collapsed="true"/>
-    <col min="108" max="108" bestFit="true" customWidth="true" style="12" width="17.0" collapsed="true"/>
-    <col min="109" max="109" bestFit="true" customWidth="true" style="12" width="16.140625" collapsed="true"/>
-    <col min="110" max="110" bestFit="true" customWidth="true" style="2" width="15.140625" collapsed="true"/>
-    <col min="111" max="111" bestFit="true" customWidth="true" style="17" width="25.28515625" collapsed="true"/>
-    <col min="112" max="112" bestFit="true" customWidth="true" style="17" width="22.5703125" collapsed="true"/>
-    <col min="113" max="113" bestFit="true" customWidth="true" style="2" width="18.42578125" collapsed="true"/>
-    <col min="114" max="114" bestFit="true" customWidth="true" style="2" width="17.28515625" collapsed="true"/>
-    <col min="115" max="115" bestFit="true" customWidth="true" style="2" width="16.140625" collapsed="true"/>
-    <col min="116" max="116" customWidth="true" style="1" width="14.0" collapsed="true"/>
-    <col min="117" max="117" bestFit="true" customWidth="true" style="1" width="15.85546875" collapsed="true"/>
-    <col min="118" max="118" bestFit="true" customWidth="true" style="12" width="12.0" collapsed="true"/>
-    <col min="119" max="119" bestFit="true" customWidth="true" style="1" width="12.7109375" collapsed="true"/>
-    <col min="120" max="120" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
-    <col min="121" max="121" bestFit="true" customWidth="true" style="1" width="11.0" collapsed="true"/>
-    <col min="122" max="122" bestFit="true" customWidth="true" style="1" width="16.85546875" collapsed="true"/>
-    <col min="123" max="123" bestFit="true" customWidth="true" style="1" width="13.28515625" collapsed="true"/>
-    <col min="124" max="124" bestFit="true" customWidth="true" style="1" width="13.140625" collapsed="true"/>
-    <col min="125" max="125" bestFit="true" customWidth="true" style="1" width="10.5703125" collapsed="true"/>
-    <col min="126" max="126" bestFit="true" customWidth="true" style="1" width="15.140625" collapsed="true"/>
-    <col min="127" max="127" bestFit="true" customWidth="true" style="1" width="19.7109375" collapsed="true"/>
-    <col min="128" max="128" bestFit="true" customWidth="true" style="1" width="22.7109375" collapsed="true"/>
-    <col min="129" max="129" bestFit="true" customWidth="true" style="1" width="29.0" collapsed="true"/>
-    <col min="130" max="130" bestFit="true" customWidth="true" style="1" width="23.7109375" collapsed="true"/>
-    <col min="131" max="131" bestFit="true" customWidth="true" style="1" width="16.42578125" collapsed="true"/>
-    <col min="132" max="132" bestFit="true" customWidth="true" style="1" width="23.5703125" collapsed="true"/>
-    <col min="133" max="133" bestFit="true" customWidth="true" style="1" width="20.5703125" collapsed="true"/>
-    <col min="134" max="134" bestFit="true" customWidth="true" style="1" width="27.42578125" collapsed="true"/>
-    <col min="135" max="135" bestFit="true" customWidth="true" style="1" width="25.85546875" collapsed="true"/>
-    <col min="136" max="136" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
-    <col min="137" max="137" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
-    <col min="138" max="138" bestFit="true" customWidth="true" style="21" width="20.7109375" collapsed="true"/>
-    <col min="139" max="139" bestFit="true" customWidth="true" style="1" width="24.5703125" collapsed="true"/>
-    <col min="140" max="140" bestFit="true" customWidth="true" style="1" width="13.42578125" collapsed="true"/>
-    <col min="141" max="141" bestFit="true" customWidth="true" style="1" width="18.28515625" collapsed="true"/>
-    <col min="142" max="143" bestFit="true" customWidth="true" style="1" width="21.140625" collapsed="true"/>
-    <col min="144" max="144" customWidth="true" style="1" width="21.140625" collapsed="true"/>
-    <col min="145" max="145" bestFit="true" customWidth="true" style="1" width="26.5703125" collapsed="true"/>
-    <col min="146" max="146" bestFit="true" customWidth="true" style="1" width="20.5703125" collapsed="true"/>
-    <col min="147" max="147" customWidth="true" style="1" width="26.28515625" collapsed="true"/>
-    <col min="148" max="148" bestFit="true" customWidth="true" style="1" width="23.85546875" collapsed="true"/>
-    <col min="149" max="149" bestFit="true" customWidth="true" style="1" width="22.7109375" collapsed="true"/>
-    <col min="150" max="150" bestFit="true" customWidth="true" style="1" width="31.85546875" collapsed="true"/>
-    <col min="151" max="151" bestFit="true" customWidth="true" style="1" width="15.140625" collapsed="true"/>
-    <col min="152" max="152" bestFit="true" customWidth="true" style="1" width="13.28515625" collapsed="true"/>
-    <col min="153" max="153" bestFit="true" customWidth="true" style="12" width="27.85546875" collapsed="true"/>
-    <col min="154" max="154" bestFit="true" customWidth="true" style="1" width="12.85546875" collapsed="true"/>
-    <col min="155" max="155" bestFit="true" customWidth="true" style="1" width="18.5703125" collapsed="true"/>
-    <col min="156" max="156" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
-    <col min="157" max="157" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
-    <col min="158" max="158" bestFit="true" customWidth="true" style="1" width="17.5703125" collapsed="true"/>
-    <col min="159" max="159" bestFit="true" customWidth="true" style="1" width="16.28515625" collapsed="true"/>
-    <col min="160" max="160" bestFit="true" customWidth="true" style="1" width="16.140625" collapsed="true"/>
-    <col min="161" max="161" bestFit="true" customWidth="true" style="1" width="14.5703125" collapsed="true"/>
-    <col min="162" max="162" customWidth="true" style="1" width="16.5703125" collapsed="true"/>
-    <col min="163" max="163" customWidth="true" style="1" width="9.140625" collapsed="true"/>
-    <col min="164" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="12.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="47.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="47.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="32.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="21" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="21" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="19" width="39" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="28.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="23" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="19.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="18.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="22.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="14.7109375" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="28" width="12.7109375" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="29" max="29" width="10.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="30" max="30" width="19.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="31" max="31" width="11.85546875" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="12.7109375" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="14.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="19.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="17.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="37" width="14.140625" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="16.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="11.140625" style="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="9.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="10.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="14.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="18.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="20.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="12.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="21.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="48" width="9.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="16.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="14.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="19.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="21" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="17.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="10.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="15.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="14.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="58" max="58" width="19" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="59" max="59" width="18.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="60" max="60" width="19.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="61" max="61" width="19.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="62" max="62" width="22.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="63" max="64" width="9.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="65" max="65" width="12.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="66" max="66" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="67" max="67" width="14.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="68" max="68" width="13" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="69" max="69" width="19.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="70" max="70" width="22.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="71" max="71" width="17.28515625" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="72" max="72" width="15.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="73" max="73" width="14.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="74" max="74" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="75" max="75" width="14.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="76" max="76" width="11.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="77" max="77" width="11.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="78" max="78" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="79" max="79" width="10.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="80" max="80" width="22.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="81" max="81" width="25.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="82" max="82" width="14.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="83" max="83" width="13.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="84" max="86" width="30.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="87" max="87" width="22.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="88" max="88" width="39" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="89" max="89" width="14.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="90" max="90" width="17.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="91" max="91" width="27.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="92" max="92" width="31.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="93" max="93" width="24.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="94" max="94" width="9.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="95" max="95" width="17.140625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="96" max="96" width="15.5703125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="97" max="97" width="24" style="1" customWidth="1" collapsed="1"/>
+    <col min="98" max="98" width="24.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="99" max="99" width="21.42578125" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="100" max="100" width="19.7109375" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="101" max="101" width="15.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="102" max="102" width="13.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="103" max="103" width="39.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="104" max="104" width="12.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="105" max="105" width="14.42578125" style="2" customWidth="1" collapsed="1"/>
+    <col min="106" max="106" width="15.5703125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="107" max="107" width="19.85546875" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="108" max="108" width="17" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="109" max="109" width="16.140625" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="110" max="110" width="15.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="111" max="111" width="25.28515625" style="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="112" max="112" width="22.5703125" style="17" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="113" max="113" width="18.42578125" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="114" max="114" width="17.28515625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="115" max="115" width="16.140625" style="2" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="116" max="116" width="14" style="1" customWidth="1" collapsed="1"/>
+    <col min="117" max="117" width="15.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="118" max="118" width="12" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="119" max="119" width="12.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="120" max="120" width="9.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="121" max="121" width="11" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="122" max="122" width="16.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="123" max="123" width="13.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="124" max="124" width="13.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="125" max="125" width="10.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="126" max="126" width="15.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="127" max="127" width="19.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="128" max="128" width="22.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="129" max="129" width="29" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="130" max="130" width="23.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="131" max="131" width="16.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="132" max="132" width="23.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="133" max="133" width="20.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="134" max="134" width="27.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="135" max="135" width="25.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="136" max="136" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="137" max="137" width="15.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="138" max="138" width="20.7109375" style="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="139" max="139" width="24.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="140" max="140" width="13.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="141" max="141" width="18.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="142" max="143" width="21.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="144" max="144" width="21.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="145" max="145" width="26.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="146" max="146" width="20.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="147" max="147" width="26.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="148" max="148" width="23.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="149" max="149" width="22.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="150" max="150" width="31.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="151" max="151" width="15.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="152" max="152" width="13.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="153" max="153" width="27.85546875" style="12" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="154" max="154" width="12.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="155" max="155" width="18.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="156" max="156" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="157" max="157" width="11.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="158" max="158" width="17.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="159" max="159" width="16.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="160" max="160" width="16.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="161" max="161" width="14.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="162" max="162" width="16.5703125" style="1" customWidth="1" collapsed="1"/>
+    <col min="163" max="163" width="9.140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="164" max="16384" width="9.140625" style="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:162" s="5" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1903,7 +1795,7 @@
         <v>166</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>167</v>
@@ -1976,106 +1868,106 @@
         <v>181</v>
       </c>
       <c r="AM2" s="10" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
       <c r="AN2" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="AR2" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="AR2" s="1" t="s">
+      <c r="AS2" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="AS2" s="1" t="s">
+      <c r="AT2" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="AT2" s="1" t="s">
+      <c r="AW2" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="AW2" s="1" t="s">
+      <c r="AX2" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="AY2" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="AX2" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="AY2" s="1" t="s">
+      <c r="AZ2" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="AZ2" s="1" t="s">
+      <c r="BA2" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="BA2" s="1" t="s">
+      <c r="BB2" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="BB2" s="1" t="s">
+      <c r="BG2" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BG2" s="1" t="s">
+      <c r="BH2" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="BJ2" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="BH2" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="BJ2" s="1" t="s">
+      <c r="BO2" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="BO2" s="1" t="s">
+      <c r="BQ2" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="BQ2" s="1" t="s">
+      <c r="BR2" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="BT2" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="BR2" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="BT2" s="1" t="s">
-        <v>196</v>
       </c>
       <c r="BV2" s="1">
         <v>1</v>
       </c>
       <c r="BW2" s="22" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="BX2" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="BY2" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="BY2" s="1" t="s">
+      <c r="BZ2" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="CA2" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="BZ2" s="22" t="s">
-        <v>213</v>
-      </c>
-      <c r="CA2" s="1" t="s">
+      <c r="CB2" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="CB2" s="1" t="s">
+      <c r="CC2" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="CC2" s="1" t="s">
+      <c r="CD2" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="CD2" s="1" t="s">
+      <c r="CE2" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="CE2" s="1" t="s">
+      <c r="CF2" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="CF2" s="1" t="s">
-        <v>204</v>
-      </c>
       <c r="CG2" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="CH2" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="CJ2" s="1" t="s">
         <v>173</v>
       </c>
       <c r="CK2" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="CL2" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="CL2" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="CP2" s="3">
         <v>1</v>
@@ -2099,49 +1991,49 @@
         <v>3975.6923076923076</v>
       </c>
       <c r="CW2" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="CZ2" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="DA2" s="2" t="s">
         <v>182</v>
       </c>
       <c r="DC2" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="DF2" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="DK2" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="DL2" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="DM2" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="DN2" s="23" t="s">
+        <v>211</v>
+      </c>
+      <c r="DO2" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="DM2" s="22" t="s">
-        <v>211</v>
-      </c>
-      <c r="DN2" s="23" t="s">
-        <v>212</v>
-      </c>
-      <c r="DO2" s="1" t="s">
+      <c r="DP2" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="DP2" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="DQ2" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="DR2" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="DS2" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="DU2" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:162" x14ac:dyDescent="0.25">
@@ -2161,7 +2053,7 @@
         <v>166</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>167</v>
@@ -2233,106 +2125,106 @@
         <v>181</v>
       </c>
       <c r="AM3" s="10" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
       <c r="AN3" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="AR3" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="AR3" s="1" t="s">
+      <c r="AS3" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="AS3" s="1" t="s">
+      <c r="AT3" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="AT3" s="1" t="s">
+      <c r="AW3" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="AW3" s="1" t="s">
+      <c r="AX3" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="AY3" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="AX3" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="AY3" s="1" t="s">
+      <c r="AZ3" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="AZ3" s="1" t="s">
+      <c r="BA3" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="BA3" s="1" t="s">
+      <c r="BB3" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="BB3" s="1" t="s">
+      <c r="BG3" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="BG3" s="1" t="s">
+      <c r="BH3" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="BJ3" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="BH3" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="BJ3" s="1" t="s">
-        <v>193</v>
-      </c>
       <c r="BO3" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="BQ3" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="BR3" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="BT3" s="1" t="s">
         <v>195</v>
-      </c>
-      <c r="BR3" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="BT3" s="1" t="s">
-        <v>196</v>
       </c>
       <c r="BV3" s="1">
         <v>1</v>
       </c>
       <c r="BW3" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="BX3" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="BY3" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="BY3" s="1" t="s">
+      <c r="BZ3" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="CA3" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="BZ3" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="CA3" s="1" t="s">
+      <c r="CB3" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="CB3" s="1" t="s">
+      <c r="CC3" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="CC3" s="1" t="s">
+      <c r="CD3" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="CD3" s="1" t="s">
+      <c r="CE3" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="CE3" s="1" t="s">
+      <c r="CF3" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="CF3" s="1" t="s">
-        <v>204</v>
-      </c>
       <c r="CG3" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="CH3" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="CJ3" s="1" t="s">
         <v>173</v>
       </c>
       <c r="CK3" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="CL3" s="1" t="s">
         <v>205</v>
-      </c>
-      <c r="CL3" s="1" t="s">
-        <v>206</v>
       </c>
       <c r="CP3" s="3">
         <v>1</v>
@@ -2356,49 +2248,49 @@
         <v>3975.6923076923076</v>
       </c>
       <c r="CW3" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="CZ3" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="DA3" s="2" t="s">
         <v>182</v>
       </c>
       <c r="DC3" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="DF3" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="DK3" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="DL3" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="DM3" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="DN3" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="DO3" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="DM3" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="DN3" s="12" t="s">
-        <v>212</v>
-      </c>
-      <c r="DO3" s="1" t="s">
+      <c r="DP3" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="DP3" s="1" t="s">
-        <v>210</v>
-      </c>
       <c r="DQ3" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="DR3" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="DS3" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="DU3" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>